<commit_message>
Update labels for variables
</commit_message>
<xml_diff>
--- a/data/cultivar_data_2019-2023_May6.xlsx
+++ b/data/cultivar_data_2019-2023_May6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanvazquez/Documents/GitHub/UARPP_Dashboard2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FEAEB47-ED7C-4C40-985D-82B08F06BE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC65C353-A916-A64C-A63D-BDC2065DE188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28760" yWindow="-1540" windowWidth="38400" windowHeight="21100" xr2:uid="{61771A6E-A3CA-432D-90F9-F5CF5B3FC66F}"/>
+    <workbookView xWindow="28800" yWindow="-1540" windowWidth="38400" windowHeight="21100" xr2:uid="{61771A6E-A3CA-432D-90F9-F5CF5B3FC66F}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -54,18 +54,6 @@
   </si>
   <si>
     <t>HMC-AM5200</t>
-  </si>
-  <si>
-    <t>Peak</t>
-  </si>
-  <si>
-    <t>Trough</t>
-  </si>
-  <si>
-    <t>Breakdown</t>
-  </si>
-  <si>
-    <t>Setback</t>
   </si>
   <si>
     <t>Pureline</t>
@@ -177,36 +165,6 @@
   </si>
   <si>
     <t>DG263L</t>
-  </si>
-  <si>
-    <t>MRY_10s</t>
-  </si>
-  <si>
-    <t>MRY_15s</t>
-  </si>
-  <si>
-    <t>MRY_20s</t>
-  </si>
-  <si>
-    <t>MRY_30s</t>
-  </si>
-  <si>
-    <t>MRY_40s</t>
-  </si>
-  <si>
-    <t>HRY_10s</t>
-  </si>
-  <si>
-    <t>HRY_15s</t>
-  </si>
-  <si>
-    <t>HRY_20s</t>
-  </si>
-  <si>
-    <t>HRY_30s</t>
-  </si>
-  <si>
-    <t>HRY_40s</t>
   </si>
   <si>
     <t>SLC_10s</t>
@@ -329,18 +287,6 @@
     <t>HCM_b_40s</t>
   </si>
   <si>
-    <t>Final</t>
-  </si>
-  <si>
-    <t>PeakTime</t>
-  </si>
-  <si>
-    <t>PastingTemp</t>
-  </si>
-  <si>
-    <t>Wbrown_Chalk</t>
-  </si>
-  <si>
     <t>Wbrown_Length</t>
   </si>
   <si>
@@ -351,12 +297,6 @@
   </si>
   <si>
     <t>Protein</t>
-  </si>
-  <si>
-    <t>FieldFissures</t>
-  </si>
-  <si>
-    <t>PurelineHybrid</t>
   </si>
   <si>
     <t>Note</t>
@@ -447,6 +387,66 @@
   </si>
   <si>
     <t>Gemini</t>
+  </si>
+  <si>
+    <t>Peak Viscosity</t>
+  </si>
+  <si>
+    <t>Trough Viscosity</t>
+  </si>
+  <si>
+    <t>Breakdown Viscosity</t>
+  </si>
+  <si>
+    <t>Final Viscosity</t>
+  </si>
+  <si>
+    <t>Setback Viscosity</t>
+  </si>
+  <si>
+    <t>Pasting Temperature</t>
+  </si>
+  <si>
+    <t>Peak Time</t>
+  </si>
+  <si>
+    <t>Field Fissures</t>
+  </si>
+  <si>
+    <t>Pureline Hybrid</t>
+  </si>
+  <si>
+    <t>Head Rice Yield_10s</t>
+  </si>
+  <si>
+    <t>Head Rice Yield_15s</t>
+  </si>
+  <si>
+    <t>Head Rice Yield_20s</t>
+  </si>
+  <si>
+    <t>Head Rice Yield_30s</t>
+  </si>
+  <si>
+    <t>Head Rice Yield_40s</t>
+  </si>
+  <si>
+    <t>Windseedle Brown Rice Chalkiness</t>
+  </si>
+  <si>
+    <t>Milled Rice Yield_10s</t>
+  </si>
+  <si>
+    <t>Milled Rice Yield_15s</t>
+  </si>
+  <si>
+    <t>Milled Rice Yield_20s</t>
+  </si>
+  <si>
+    <t>Milled Rice Yield_30s</t>
+  </si>
+  <si>
+    <t>Milled Rice Yield_40s</t>
   </si>
 </sst>
 </file>
@@ -963,9 +963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4D1261-57B9-4837-9D88-61377C47FD54}">
   <dimension ref="A1:BR177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B171" sqref="B171"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -984,10 +984,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>2</v>
@@ -999,193 +999,193 @@
         <v>4</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="L1" s="24" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="N1" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="U1" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="W1" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="AC1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="AD1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="AE1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="AF1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="24" t="s">
+      <c r="AG1" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="AH1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="AI1" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="AJ1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="AK1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="AL1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" s="25" t="s">
+      <c r="AM1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="AN1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AO1" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AP1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AQ1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AR1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" s="25" t="s">
+      <c r="AS1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="25" t="s">
+      <c r="AT1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="AG1" s="25" t="s">
+      <c r="AU1" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="25" t="s">
+      <c r="AV1" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="AI1" s="25" t="s">
+      <c r="AW1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="AJ1" s="25" t="s">
+      <c r="AX1" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="25" t="s">
+      <c r="AY1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="AL1" s="25" t="s">
+      <c r="AZ1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="AM1" s="25" t="s">
+      <c r="BA1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="AN1" s="25" t="s">
+      <c r="BB1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AO1" s="25" t="s">
+      <c r="BC1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AP1" s="25" t="s">
+      <c r="BD1" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="BE1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="AR1" s="25" t="s">
+      <c r="BF1" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="AS1" s="25" t="s">
+      <c r="BG1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="AT1" s="25" t="s">
+      <c r="BH1" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="AU1" s="25" t="s">
+      <c r="BI1" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="25" t="s">
+      <c r="BJ1" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="AW1" s="25" t="s">
+      <c r="BK1" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="AX1" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="AY1" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ1" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="BA1" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="BB1" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="BC1" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="BD1" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE1" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="BF1" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="BG1" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="BH1" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="BI1" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ1" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="BK1" s="25" t="s">
-        <v>95</v>
-      </c>
       <c r="BL1" s="26" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="BM1" s="26" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="BN1" s="26" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="BO1" s="26" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="BP1" s="26" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="BQ1" s="26" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="BR1" s="26" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.2">
@@ -1193,14 +1193,14 @@
         <v>2022</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1">
         <v>16</v>
@@ -1400,14 +1400,14 @@
         <v>2022</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1">
         <v>19.2</v>
@@ -1607,13 +1607,13 @@
         <v>2023</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H4" s="14">
         <v>27</v>
@@ -1747,13 +1747,13 @@
         <v>2019</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4">
         <v>16.3</v>
@@ -1956,13 +1956,13 @@
         <v>2021</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" s="1">
         <v>16.5</v>
@@ -2165,13 +2165,13 @@
         <v>2020</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2">
         <v>16.5</v>
@@ -2329,13 +2329,13 @@
         <v>2020</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2">
         <v>17.5</v>
@@ -2493,13 +2493,13 @@
         <v>2022</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1">
         <v>24.7</v>
@@ -2699,14 +2699,14 @@
         <v>2022</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G10" s="1">
         <v>24</v>
@@ -2906,13 +2906,13 @@
         <v>2021</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1">
         <v>19.2</v>
@@ -3115,13 +3115,13 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F12" s="2">
         <v>17.600000000000001</v>
@@ -3261,13 +3261,13 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F13" s="2">
         <v>17.8</v>
@@ -3407,13 +3407,13 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H14" s="10">
         <v>22</v>
@@ -3547,13 +3547,13 @@
         <v>2020</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F15" s="2">
         <v>14.5</v>
@@ -3711,13 +3711,13 @@
         <v>2020</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F16" s="2">
         <v>12.7</v>
@@ -3875,13 +3875,13 @@
         <v>2019</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="4">
@@ -4082,13 +4082,13 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H18" s="10">
         <v>34</v>
@@ -4222,13 +4222,13 @@
         <v>2022</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G19" s="1">
         <v>20.2</v>
@@ -4428,13 +4428,13 @@
         <v>2022</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G20" s="1">
         <v>21.4</v>
@@ -4634,13 +4634,13 @@
         <v>2021</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F21" s="1">
         <v>18.899999999999999</v>
@@ -4843,13 +4843,13 @@
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H22" s="10">
         <v>25</v>
@@ -4983,13 +4983,13 @@
         <v>2020</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G23" s="1">
         <v>17.5</v>
@@ -5141,13 +5141,13 @@
         <v>2019</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F24" s="4">
         <v>18</v>
@@ -5350,13 +5350,13 @@
         <v>2019</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F25" s="4">
         <v>19.399999999999999</v>
@@ -5559,16 +5559,16 @@
         <v>2020</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F26" s="2">
         <v>15.3</v>
@@ -5726,16 +5726,16 @@
         <v>2020</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F27" s="2">
         <v>15.7</v>
@@ -5893,16 +5893,16 @@
         <v>2020</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F28" s="2">
         <v>17</v>
@@ -6060,16 +6060,16 @@
         <v>2020</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F29" s="2">
         <v>17.600000000000001</v>
@@ -6227,16 +6227,16 @@
         <v>2020</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F30" s="2">
         <v>18.8</v>
@@ -6388,16 +6388,16 @@
         <v>2020</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F31" s="2">
         <v>15.8</v>
@@ -6555,16 +6555,16 @@
         <v>2020</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F32" s="2">
         <v>13.9</v>
@@ -6722,16 +6722,16 @@
         <v>2020</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F33" s="2">
         <v>15.3</v>
@@ -6889,16 +6889,16 @@
         <v>2020</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F34" s="2">
         <v>15.8</v>
@@ -7056,16 +7056,16 @@
         <v>2020</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F35" s="2">
         <v>16.399999999999999</v>
@@ -7223,16 +7223,16 @@
         <v>2019</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F36" s="4">
         <v>16</v>
@@ -7435,16 +7435,16 @@
         <v>2021</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F37" s="1">
         <v>17.399999999999999</v>
@@ -7647,14 +7647,14 @@
         <v>2022</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G38" s="1">
         <v>18.5</v>
@@ -7854,14 +7854,14 @@
         <v>2022</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G39" s="1">
         <v>18.5</v>
@@ -8059,13 +8059,13 @@
         <v>2023</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F40" s="2">
         <v>16.5</v>
@@ -8205,13 +8205,13 @@
         <v>2023</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F41" s="2">
         <v>16</v>
@@ -8351,13 +8351,13 @@
         <v>2023</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H42" s="17"/>
       <c r="I42" s="4">
@@ -8489,16 +8489,16 @@
         <v>2023</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H43" s="10">
         <v>60</v>
@@ -8632,13 +8632,13 @@
         <v>2021</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F44" s="1">
         <v>18.3</v>
@@ -8841,14 +8841,14 @@
         <v>2022</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G45" s="1">
         <v>21.8</v>
@@ -9048,14 +9048,14 @@
         <v>2022</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G46" s="1">
         <v>19.5</v>
@@ -9255,13 +9255,13 @@
         <v>2023</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F47" s="2">
         <v>14.2</v>
@@ -9401,13 +9401,13 @@
         <v>2023</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F48" s="2">
         <v>15.5</v>
@@ -9547,16 +9547,16 @@
         <v>2019</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F49" s="4">
         <v>14.4</v>
@@ -9759,16 +9759,16 @@
         <v>2019</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F50" s="4">
         <v>14.6</v>
@@ -9971,14 +9971,14 @@
         <v>2022</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G51" s="1">
         <v>16.100000000000001</v>
@@ -10176,14 +10176,14 @@
         <v>2022</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G52" s="1">
         <v>16.100000000000001</v>
@@ -10383,13 +10383,13 @@
         <v>2023</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F53" s="2">
         <v>14.7</v>
@@ -10529,16 +10529,16 @@
         <v>2019</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F54" s="4">
         <v>14.1</v>
@@ -10741,16 +10741,16 @@
         <v>2019</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F55" s="4">
         <v>14.5</v>
@@ -10953,16 +10953,16 @@
         <v>2023</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F56" s="2">
         <v>14.1</v>
@@ -11102,16 +11102,16 @@
         <v>2023</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F57" s="2">
         <v>10.199999999999999</v>
@@ -11251,16 +11251,16 @@
         <v>2022</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G58" s="1">
         <v>15.9</v>
@@ -11460,16 +11460,16 @@
         <v>2022</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G59" s="1">
         <v>15.3</v>
@@ -11669,13 +11669,13 @@
         <v>2022</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G60" s="1">
         <v>16.399999999999999</v>
@@ -11875,13 +11875,13 @@
         <v>2022</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G61" s="1">
         <v>14.6</v>
@@ -12081,13 +12081,13 @@
         <v>2020</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F62" s="2">
         <v>14</v>
@@ -12245,13 +12245,13 @@
         <v>2019</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F63" s="4">
         <v>15.2</v>
@@ -12454,13 +12454,13 @@
         <v>2019</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F64" s="4">
         <v>16.5</v>
@@ -12663,13 +12663,13 @@
         <v>2023</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F65" s="2">
         <v>16.3</v>
@@ -12809,16 +12809,16 @@
         <v>2021</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F66" s="1">
         <v>16.600000000000001</v>
@@ -13021,16 +13021,16 @@
         <v>2021</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F67" s="1">
         <v>16.8</v>
@@ -13233,16 +13233,16 @@
         <v>2021</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F68" s="1">
         <v>16.2</v>
@@ -13445,13 +13445,13 @@
         <v>2023</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F69" s="2">
         <v>16.8</v>
@@ -13591,13 +13591,13 @@
         <v>2023</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F70" s="2">
         <v>16.5</v>
@@ -13737,13 +13737,13 @@
         <v>2019</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F71" s="4">
         <v>15.9</v>
@@ -13946,16 +13946,16 @@
         <v>2022</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G72" s="1">
         <v>15.4</v>
@@ -14155,16 +14155,16 @@
         <v>2022</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G73" s="1">
         <v>15.7</v>
@@ -14364,16 +14364,16 @@
         <v>2021</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F74" s="1">
         <v>18.600000000000001</v>
@@ -14576,16 +14576,16 @@
         <v>2019</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F75" s="4">
         <v>16.5</v>
@@ -14788,16 +14788,16 @@
         <v>2019</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F76" s="4">
         <v>14.1</v>
@@ -15000,16 +15000,16 @@
         <v>2023</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F77" s="2">
         <v>14.5</v>
@@ -15149,16 +15149,16 @@
         <v>2023</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F78" s="2">
         <v>10.6</v>
@@ -15298,16 +15298,16 @@
         <v>2021</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F79" s="1">
         <v>16.5</v>
@@ -15510,16 +15510,16 @@
         <v>2021</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F80" s="1">
         <v>17</v>
@@ -15722,16 +15722,16 @@
         <v>2019</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F81" s="4">
         <v>13.8</v>
@@ -15934,16 +15934,16 @@
         <v>2019</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F82" s="4">
         <v>14.2</v>
@@ -16146,16 +16146,16 @@
         <v>2022</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G83" s="1">
         <v>15</v>
@@ -16355,16 +16355,16 @@
         <v>2022</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G84" s="1">
         <v>14.5</v>
@@ -16564,16 +16564,16 @@
         <v>2021</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1">
         <v>16</v>
@@ -16776,16 +16776,16 @@
         <v>2023</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F86" s="2">
         <v>15.1</v>
@@ -16925,16 +16925,16 @@
         <v>2023</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F87" s="2">
         <v>11.4</v>
@@ -17074,13 +17074,13 @@
         <v>2022</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
         <v>15.7</v>
@@ -17280,13 +17280,13 @@
         <v>2022</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
         <v>17.2</v>
@@ -17486,13 +17486,13 @@
         <v>2020</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F90" s="1">
         <v>15.6</v>
@@ -17650,13 +17650,13 @@
         <v>2023</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F91" s="2">
         <v>18.3</v>
@@ -17796,13 +17796,13 @@
         <v>2023</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F92" s="2">
         <v>15.8</v>
@@ -17942,16 +17942,16 @@
         <v>2021</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F93" s="1">
         <v>16.7</v>
@@ -18154,16 +18154,16 @@
         <v>2022</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G94" s="1">
         <v>17</v>
@@ -18363,16 +18363,16 @@
         <v>2022</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G95" s="1">
         <v>17.100000000000001</v>
@@ -18572,16 +18572,16 @@
         <v>2023</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F96" s="2">
         <v>15.4</v>
@@ -18721,16 +18721,16 @@
         <v>2023</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F97" s="2">
         <v>13.4</v>
@@ -18870,16 +18870,16 @@
         <v>2021</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F98" s="1">
         <v>17.2</v>
@@ -19080,16 +19080,16 @@
         <v>2022</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G99" s="1">
         <v>16.5</v>
@@ -19289,16 +19289,16 @@
         <v>2022</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G100" s="1">
         <v>15.8</v>
@@ -19498,16 +19498,16 @@
         <v>2023</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F101" s="2">
         <v>13.7</v>
@@ -19647,16 +19647,16 @@
         <v>2023</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F102" s="2">
         <v>15.5</v>
@@ -19796,13 +19796,13 @@
         <v>2020</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G103" s="1">
         <v>16.8</v>
@@ -19954,13 +19954,13 @@
         <v>2019</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F104" s="4">
         <v>15.9</v>
@@ -20163,13 +20163,13 @@
         <v>2019</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F105" s="4">
         <v>16.2</v>
@@ -20372,13 +20372,13 @@
         <v>2022</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G106" s="1">
         <v>17.5</v>
@@ -20578,16 +20578,16 @@
         <v>2022</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G107" s="1">
         <v>18.2</v>
@@ -20787,16 +20787,16 @@
         <v>2021</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F108" s="1">
         <v>16.5</v>
@@ -20999,16 +20999,16 @@
         <v>2019</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F109" s="4">
         <v>17</v>
@@ -21205,16 +21205,16 @@
         <v>2019</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F110" s="4">
         <v>16.5</v>
@@ -21417,16 +21417,16 @@
         <v>2023</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F111" s="2">
         <v>15.3</v>
@@ -21566,16 +21566,16 @@
         <v>2023</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F112" s="2">
         <v>12.8</v>
@@ -21715,16 +21715,16 @@
         <v>2021</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F113" s="1">
         <v>16.5</v>
@@ -21927,16 +21927,16 @@
         <v>2021</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F114" s="1">
         <v>17.7</v>
@@ -22139,16 +22139,16 @@
         <v>2022</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G115" s="1">
         <v>16.2</v>
@@ -22348,16 +22348,16 @@
         <v>2022</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G116" s="1">
         <v>17.3</v>
@@ -22557,16 +22557,16 @@
         <v>2023</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F117" s="2">
         <v>13.5</v>
@@ -22706,16 +22706,16 @@
         <v>2023</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F118" s="2">
         <v>15.7</v>
@@ -22855,16 +22855,16 @@
         <v>2021</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F119" s="1">
         <v>17.5</v>
@@ -23067,13 +23067,13 @@
         <v>2020</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G120" s="1">
         <v>17.2</v>
@@ -23225,13 +23225,13 @@
         <v>2019</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F121" s="4">
         <v>17.399999999999999</v>
@@ -23434,13 +23434,13 @@
         <v>2019</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F122" s="4">
         <v>18.600000000000001</v>
@@ -23643,16 +23643,16 @@
         <v>2021</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F123" s="1">
         <v>16.3</v>
@@ -23855,16 +23855,16 @@
         <v>2023</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F124" s="2">
         <v>13.4</v>
@@ -24004,16 +24004,16 @@
         <v>2023</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F125" s="2">
         <v>11.5</v>
@@ -24153,13 +24153,13 @@
         <v>2022</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G126" s="1">
         <v>17.399999999999999</v>
@@ -24359,13 +24359,13 @@
         <v>2022</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G127" s="1">
         <v>17.2</v>
@@ -24565,13 +24565,13 @@
         <v>2023</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F128" s="2">
         <v>18.5</v>
@@ -24711,13 +24711,13 @@
         <v>2023</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F129" s="2">
         <v>15.9</v>
@@ -24857,13 +24857,13 @@
         <v>2021</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F130" s="1">
         <v>22.5</v>
@@ -25064,13 +25064,13 @@
         <v>2019</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F131" s="4">
         <v>15.3</v>
@@ -25273,13 +25273,13 @@
         <v>2019</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F132" s="4">
         <v>15.6</v>
@@ -25482,13 +25482,13 @@
         <v>2023</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F133" s="2">
         <v>14.2</v>
@@ -25628,13 +25628,13 @@
         <v>2023</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F134" s="2">
         <v>16.899999999999999</v>
@@ -25774,16 +25774,16 @@
         <v>2021</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F135" s="1">
         <v>16.899999999999999</v>
@@ -25986,16 +25986,16 @@
         <v>2021</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F136" s="1">
         <v>16.600000000000001</v>
@@ -26198,13 +26198,13 @@
         <v>2022</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G137" s="1">
         <v>18.100000000000001</v>
@@ -26404,13 +26404,13 @@
         <v>2022</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G138" s="1">
         <v>19.2</v>
@@ -26610,16 +26610,16 @@
         <v>2021</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F139" s="1">
         <v>17.600000000000001</v>
@@ -26822,16 +26822,16 @@
         <v>2019</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F140" s="4">
         <v>15.2</v>
@@ -27034,16 +27034,16 @@
         <v>2019</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F141" s="4">
         <v>14.9</v>
@@ -27246,13 +27246,13 @@
         <v>2022</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G142" s="1">
         <v>15.5</v>
@@ -27452,13 +27452,13 @@
         <v>2022</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G143" s="1">
         <v>15.2</v>
@@ -27658,13 +27658,13 @@
         <v>2021</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F144" s="1">
         <v>16.8</v>
@@ -27867,13 +27867,13 @@
         <v>2020</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F145" s="1">
         <v>18.5</v>
@@ -28031,13 +28031,13 @@
         <v>2019</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F146" s="4">
         <v>14</v>
@@ -28240,13 +28240,13 @@
         <v>2019</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F147" s="4">
         <v>14.2</v>
@@ -28449,13 +28449,13 @@
         <v>2023</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F148" s="2">
         <v>16</v>
@@ -28595,13 +28595,13 @@
         <v>2019</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F149" s="4">
         <v>14</v>
@@ -28798,13 +28798,13 @@
         <v>2019</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F150" s="4">
         <v>19</v>
@@ -29001,13 +29001,13 @@
         <v>2019</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F151" s="4">
         <v>16.100000000000001</v>
@@ -29210,13 +29210,13 @@
         <v>2019</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F152" s="4">
         <v>16.5</v>
@@ -29419,13 +29419,13 @@
         <v>2019</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F153" s="4">
         <v>16.100000000000001</v>
@@ -29628,13 +29628,13 @@
         <v>2019</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F154" s="4">
         <v>16.600000000000001</v>
@@ -29837,16 +29837,16 @@
         <v>2021</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F155" s="1">
         <v>17.5</v>
@@ -30049,13 +30049,13 @@
         <v>2021</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F156" s="1">
         <v>18.3</v>
@@ -30258,13 +30258,13 @@
         <v>2022</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G157" s="1">
         <v>18.5</v>
@@ -30464,13 +30464,13 @@
         <v>2022</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G158" s="1">
         <v>17.399999999999999</v>
@@ -30670,16 +30670,16 @@
         <v>2021</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F159" s="1">
         <v>17.8</v>
@@ -30882,13 +30882,13 @@
         <v>2022</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G160" s="1">
         <v>18.5</v>
@@ -31088,13 +31088,13 @@
         <v>2022</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G161" s="1">
         <v>18.2</v>
@@ -31294,13 +31294,13 @@
         <v>2021</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F162" s="1">
         <v>18.7</v>
@@ -31503,13 +31503,13 @@
         <v>2023</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F163" s="2">
         <v>18.3</v>
@@ -31649,13 +31649,13 @@
         <v>2023</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F164" s="2">
         <v>15.5</v>
@@ -31795,13 +31795,13 @@
         <v>2022</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G165" s="1">
         <v>17.3</v>
@@ -32001,13 +32001,13 @@
         <v>2022</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G166" s="1">
         <v>16.8</v>
@@ -32207,13 +32207,13 @@
         <v>2023</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F167" s="2">
         <v>17.8</v>
@@ -32353,13 +32353,13 @@
         <v>2023</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F168" s="2">
         <v>16</v>
@@ -32499,16 +32499,16 @@
         <v>2021</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F169" s="1">
         <v>18.7</v>
@@ -32711,13 +32711,13 @@
         <v>2023</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F170" s="2">
         <v>16.5</v>
@@ -32857,13 +32857,13 @@
         <v>2023</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F171" s="2">
         <v>15.8</v>
@@ -33003,13 +33003,13 @@
         <v>2022</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G172" s="1">
         <v>20.3</v>
@@ -33209,13 +33209,13 @@
         <v>2022</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G173" s="1">
         <v>20.2</v>
@@ -33415,13 +33415,13 @@
         <v>2023</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F174" s="2">
         <v>15.5</v>
@@ -33561,16 +33561,16 @@
         <v>2023</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F175" s="2">
         <v>16.399999999999999</v>
@@ -33710,13 +33710,13 @@
         <v>2023</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F176" s="2">
         <v>16.600000000000001</v>
@@ -33856,13 +33856,13 @@
         <v>2023</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F177" s="2">
         <v>18.100000000000001</v>

</xml_diff>